<commit_message>
#163 cambio columna apellidos usuarios
</commit_message>
<xml_diff>
--- a/public/files/estudiantes.xlsx
+++ b/public/files/estudiantes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Home\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D31C06-63B8-48FB-8323-135FFBCBDA8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7FBA774-F197-40CB-9F24-B4C9AD519B7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21960" yWindow="3150" windowWidth="15615" windowHeight="6105" xr2:uid="{7A15F88C-8367-49EE-B550-7A0A8CB1944C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7A15F88C-8367-49EE-B550-7A0A8CB1944C}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -33,10 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>names</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>email</t>
   </si>
@@ -47,18 +44,6 @@
     <t>unique_number</t>
   </si>
   <si>
-    <t>Jonathan Vasquez</t>
-  </si>
-  <si>
-    <t>Chantal Morales</t>
-  </si>
-  <si>
-    <t>Nicole Zambrano</t>
-  </si>
-  <si>
-    <t>Kevin Segovia</t>
-  </si>
-  <si>
     <t>jonathan.vasquez01@epn.edu.ec</t>
   </si>
   <si>
@@ -69,6 +54,36 @@
   </si>
   <si>
     <t>kevin.segovia@epn.edu.ec</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>last_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jonathan </t>
+  </si>
+  <si>
+    <t>Vasquez</t>
+  </si>
+  <si>
+    <t>Morales</t>
+  </si>
+  <si>
+    <t>Zambrano</t>
+  </si>
+  <si>
+    <t>Segovia</t>
+  </si>
+  <si>
+    <t>Chantal</t>
+  </si>
+  <si>
+    <t>Nicole</t>
+  </si>
+  <si>
+    <t>Kevin</t>
   </si>
 </sst>
 </file>
@@ -439,127 +454,144 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E983D588-F43F-49CA-8734-742888C176CB}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" customWidth="1"/>
-    <col min="2" max="2" width="25.5703125" customWidth="1"/>
-    <col min="3" max="3" width="31" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" customWidth="1"/>
-    <col min="5" max="6" width="11.42578125" style="2"/>
+    <col min="1" max="2" width="22.5703125" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" customWidth="1"/>
+    <col min="4" max="4" width="31" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" customWidth="1"/>
+    <col min="6" max="7" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>201410413</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E2">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3">
+        <v>201559876</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
-        <v>201410413</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2">
+      <c r="E3">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>201654983</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3">
-        <v>201559876</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3">
+      <c r="E4">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>201443258</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4">
-        <v>201654983</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4">
+      <c r="E5">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5">
-        <v>201443258</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C6" s="1"/>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C7" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C8" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C9" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C10" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C11" s="1"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C12" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D12" s="1"/>
-    </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C21" s="3"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D21" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{A2EC1359-B2CA-44A6-B810-D443F72277B9}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{AAE9651E-DF6D-4330-B542-744211286B50}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{713AADB7-9742-46CE-9612-54AD2D452A54}"/>
-    <hyperlink ref="C5" r:id="rId4" xr:uid="{884C4A9A-4EB3-4355-973C-E891C53D96A5}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{A2EC1359-B2CA-44A6-B810-D443F72277B9}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{AAE9651E-DF6D-4330-B542-744211286B50}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{713AADB7-9742-46CE-9612-54AD2D452A54}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{884C4A9A-4EB3-4355-973C-E891C53D96A5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>

</xml_diff>

<commit_message>
#125 Cargar documentos Cloudinary
</commit_message>
<xml_diff>
--- a/public/files/estudiantes.xlsx
+++ b/public/files/estudiantes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Universidad\proyectoTesis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicole\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03D9C336-86AA-4328-9027-344938917579}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F04683B-A370-4BCA-A829-3024D5120F74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{FA10416F-BFD4-45AB-9471-F5E12934BB84}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7A15F88C-8367-49EE-B550-7A0A8CB1944C}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,58 +33,73 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>career_id</t>
+  </si>
+  <si>
+    <t>unique_number</t>
+  </si>
+  <si>
+    <t>jonathan.vasquez01@epn.edu.ec</t>
+  </si>
+  <si>
+    <t>chantal.morales@epn.edu.ec</t>
+  </si>
+  <si>
+    <t>nicole.zambrano@epn.edu.ec</t>
+  </si>
+  <si>
+    <t>kevin.segovia@epn.edu.ec</t>
+  </si>
   <si>
     <t>name</t>
   </si>
   <si>
-    <t>unique_number</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>career_id</t>
-  </si>
-  <si>
-    <t>Chantal Alejandra Morales Rojas</t>
-  </si>
-  <si>
-    <t>Kevin Javier Segovia Garzón</t>
-  </si>
-  <si>
-    <t>Jonathan Israel Vasquez Vivas</t>
-  </si>
-  <si>
-    <t>Katerine Nicole Zambrano Solorzano</t>
-  </si>
-  <si>
-    <t>chantal.morales@epn.edu.ec</t>
-  </si>
-  <si>
-    <t>kevin.segovia@epn.edu.ec</t>
-  </si>
-  <si>
-    <t>jonathan.vasquez@epn.edu.ec</t>
-  </si>
-  <si>
-    <t>katerine.zambrano@epn.edu.ec</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Katerin Vanessa Puente Delgado </t>
-  </si>
-  <si>
-    <t>katerin.puente@epn.edu.ec</t>
+    <t>last_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jonathan </t>
+  </si>
+  <si>
+    <t>Vasquez</t>
+  </si>
+  <si>
+    <t>Morales</t>
+  </si>
+  <si>
+    <t>Zambrano</t>
+  </si>
+  <si>
+    <t>Segovia</t>
+  </si>
+  <si>
+    <t>Chantal</t>
+  </si>
+  <si>
+    <t>Nicole</t>
+  </si>
+  <si>
+    <t>Kevin</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -118,11 +132,13 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -437,107 +453,147 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD077B75-9729-4CF4-A42E-6074B60B82D3}">
-  <dimension ref="A1:D6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E983D588-F43F-49CA-8734-742888C176CB}">
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E2" sqref="E2:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="22.5703125" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" customWidth="1"/>
+    <col min="4" max="4" width="31" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" customWidth="1"/>
+    <col min="6" max="7" width="11.42578125" style="2"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>201410413</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="E2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3">
+        <v>201559876</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
-        <v>201720125</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="E3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>201654983</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3">
-        <v>201720123</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="E4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>201443258</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4">
-        <v>201410413</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5">
-        <v>201720112</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6">
-        <v>201720145</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6">
+      <c r="E5">
         <v>3</v>
       </c>
     </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D21" s="3"/>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{57A92DF6-6914-4E11-81E5-25E707A5E4A8}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{7ED9D232-C757-4462-A5E8-B7AA700E5499}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{A02D6F32-8911-4662-9A34-61577F7C20C2}"/>
-    <hyperlink ref="C5" r:id="rId4" xr:uid="{620BA2F9-E6E8-4368-8C48-74468173B0E9}"/>
-    <hyperlink ref="C6" r:id="rId5" xr:uid="{91918F79-D4B7-4DFA-9294-8D10F9FA4E6F}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{A2EC1359-B2CA-44A6-B810-D443F72277B9}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{AAE9651E-DF6D-4330-B542-744211286B50}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{713AADB7-9742-46CE-9612-54AD2D452A54}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{884C4A9A-4EB3-4355-973C-E891C53D96A5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>